<commit_message>
experiment ideas for final lemmas
</commit_message>
<xml_diff>
--- a/corpus/final_lemmas.xlsx
+++ b/corpus/final_lemmas.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user1\materialy\bc\reflexive-alternation-in-aphasia\corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465DF243-E3A2-4449-A7D7-B22B5302954B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D062C0-F1E4-4A86-BE9F-68E72A890C8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="plausibility" sheetId="2" r:id="rId2"/>
+    <sheet name="grammaticallity" sheetId="3" r:id="rId3"/>
+    <sheet name="insert_reflexive" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$I$1:$I$21</definedName>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="183">
   <si>
     <t>hájit</t>
   </si>
@@ -475,6 +478,108 @@
   </si>
   <si>
     <t>film, seriál, televize, scéna, snímek</t>
+  </si>
+  <si>
+    <t>high-</t>
+  </si>
+  <si>
+    <t>dědeček se probudil ze snu</t>
+  </si>
+  <si>
+    <t>budík se probudil ze snu</t>
+  </si>
+  <si>
+    <t>budík probudil dědečka ze snu</t>
+  </si>
+  <si>
+    <t>dědeček probudil budík ze snu</t>
+  </si>
+  <si>
+    <t>low-</t>
+  </si>
+  <si>
+    <t>Petr se zapsal  do sešitu</t>
+  </si>
+  <si>
+    <t>Datum se zapsal do sešitu</t>
+  </si>
+  <si>
+    <t>petr zapsal datum do sešitu</t>
+  </si>
+  <si>
+    <t>datum zapsal petra do sešitu</t>
+  </si>
+  <si>
+    <t>reflexive use</t>
+  </si>
+  <si>
+    <t>non-reflexive use</t>
+  </si>
+  <si>
+    <t>reflexivity bias</t>
+  </si>
+  <si>
+    <t>plausible use</t>
+  </si>
+  <si>
+    <t>implausible use</t>
+  </si>
+  <si>
+    <t>dalsi slovesa, ktera lze pridat</t>
+  </si>
+  <si>
+    <t>grammatical use</t>
+  </si>
+  <si>
+    <t>non-grammatical use</t>
+  </si>
+  <si>
+    <t>dědeček se probudil</t>
+  </si>
+  <si>
+    <t>dědeček probudil</t>
+  </si>
+  <si>
+    <t>budík probudil dědečka</t>
+  </si>
+  <si>
+    <t>budík se probudil dědečka</t>
+  </si>
+  <si>
+    <t>intransitive use</t>
+  </si>
+  <si>
+    <t>transitive use</t>
+  </si>
+  <si>
+    <t>petr se zapsal datum do sešitu</t>
+  </si>
+  <si>
+    <t>petr se zapsal do sešitu</t>
+  </si>
+  <si>
+    <t>petr zapsal do sešitu</t>
+  </si>
+  <si>
+    <t>reflexive needed</t>
+  </si>
+  <si>
+    <t>reflexive not needed</t>
+  </si>
+  <si>
+    <t>example sentence</t>
+  </si>
+  <si>
+    <t>dědeček _ probudil _ ze _ snu</t>
+  </si>
+  <si>
+    <t>budik _ probudil _ dědečka _ ze _ snu</t>
+  </si>
+  <si>
+    <t>petr _ zapsal _ do _ sešitu</t>
+  </si>
+  <si>
+    <t>petr _ zapsal _ datum _ do _ sešitu</t>
   </si>
 </sst>
 </file>
@@ -490,15 +595,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -506,12 +617,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1543,6 +1754,11 @@
         <v>105</v>
       </c>
     </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>55</v>
@@ -1844,6 +2060,256 @@
       <c r="K42" t="s">
         <v>127</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174360F2-0B0E-4EF1-A5CC-2464ACF992AE}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057030CB-B800-4519-95A3-3E74CCF461EF}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E30DFC-42CC-4AC5-B31A-93F0F62B75CA}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
create sentences for the experiment (sentences.csv)
</commit_message>
<xml_diff>
--- a/corpus/final_lemmas.xlsx
+++ b/corpus/final_lemmas.xlsx
@@ -8,18 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user1\materialy\bc\reflexive-alternation-in-aphasia\corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D062C0-F1E4-4A86-BE9F-68E72A890C8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574C1F8B-D8F8-43CB-B0D8-3DCAEEE796DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
-    <sheet name="plausibility" sheetId="2" r:id="rId2"/>
-    <sheet name="grammaticallity" sheetId="3" r:id="rId3"/>
-    <sheet name="insert_reflexive" sheetId="4" r:id="rId4"/>
+    <sheet name="grammaticallity" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$I$1:$I$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$I$1:$I$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="306">
   <si>
     <t>hájit</t>
   </si>
@@ -483,33 +481,12 @@
     <t>high-</t>
   </si>
   <si>
-    <t>dědeček se probudil ze snu</t>
-  </si>
-  <si>
-    <t>budík se probudil ze snu</t>
-  </si>
-  <si>
-    <t>budík probudil dědečka ze snu</t>
-  </si>
-  <si>
-    <t>dědeček probudil budík ze snu</t>
-  </si>
-  <si>
     <t>low-</t>
   </si>
   <si>
-    <t>Petr se zapsal  do sešitu</t>
-  </si>
-  <si>
-    <t>Datum se zapsal do sešitu</t>
-  </si>
-  <si>
     <t>petr zapsal datum do sešitu</t>
   </si>
   <si>
-    <t>datum zapsal petra do sešitu</t>
-  </si>
-  <si>
     <t>reflexive use</t>
   </si>
   <si>
@@ -519,12 +496,6 @@
     <t>reflexivity bias</t>
   </si>
   <si>
-    <t>plausible use</t>
-  </si>
-  <si>
-    <t>implausible use</t>
-  </si>
-  <si>
     <t>dalsi slovesa, ktera lze pridat</t>
   </si>
   <si>
@@ -561,25 +532,421 @@
     <t>petr zapsal do sešitu</t>
   </si>
   <si>
-    <t>reflexive needed</t>
-  </si>
-  <si>
-    <t>reflexive not needed</t>
-  </si>
-  <si>
-    <t>example sentence</t>
-  </si>
-  <si>
-    <t>dědeček _ probudil _ ze _ snu</t>
-  </si>
-  <si>
-    <t>budik _ probudil _ dědečka _ ze _ snu</t>
-  </si>
-  <si>
-    <t>petr _ zapsal _ do _ sešitu</t>
-  </si>
-  <si>
-    <t>petr _ zapsal _ datum _ do _ sešitu</t>
+    <t>refl-gr</t>
+  </si>
+  <si>
+    <t>refl-ngr</t>
+  </si>
+  <si>
+    <t>tr-gr</t>
+  </si>
+  <si>
+    <t>tr-ngr</t>
+  </si>
+  <si>
+    <t>Dědeček probudil vnuka v devět hodin</t>
+  </si>
+  <si>
+    <t>Úředník zaměřil pozornost na svou práci</t>
+  </si>
+  <si>
+    <t>Úředník se zaměřil pozornost na svou práci</t>
+  </si>
+  <si>
+    <t>Úředník se zaměřil na svou práci</t>
+  </si>
+  <si>
+    <t>Úředník zaměřil na svou práci</t>
+  </si>
+  <si>
+    <t>Dědeček probudil v devět hodin</t>
+  </si>
+  <si>
+    <t>Dědeček se probudil v devět hodin</t>
+  </si>
+  <si>
+    <t>otázky</t>
+  </si>
+  <si>
+    <t>stálost gram. funkce (např. dědeček je vždy podmětem)</t>
+  </si>
+  <si>
+    <t>Dispečer vypravil vlak do Prahy</t>
+  </si>
+  <si>
+    <t>Dispečer se vypravil vlak do Prahy</t>
+  </si>
+  <si>
+    <t>Dispečer se vypravil do Prahy</t>
+  </si>
+  <si>
+    <t>Dispečer vypravil do Prahy</t>
+  </si>
+  <si>
+    <t>stejná podoba ostatních větných členů? (např jedna PP)</t>
+  </si>
+  <si>
+    <t>Tatínek přestěhoval nábytek z bytu (do chalupy)</t>
+  </si>
+  <si>
+    <t>Tatínek se přestěhoval nábytek z bytu (do chalupy)</t>
+  </si>
+  <si>
+    <t>Tatínek se přestěhoval z bytu</t>
+  </si>
+  <si>
+    <t>Tatínek přestěhoval z bytu</t>
+  </si>
+  <si>
+    <t>Učitel se omluvil na hodině</t>
+  </si>
+  <si>
+    <t>Učitel omluvil na hodině</t>
+  </si>
+  <si>
+    <t>Učitel omluvil nepřítomnost (studenta) na hodině</t>
+  </si>
+  <si>
+    <t>Učitel se omluvil nepřítomnost (studenta) na hodině</t>
+  </si>
+  <si>
+    <t>Kuchař se naklonil nad umyvadlo</t>
+  </si>
+  <si>
+    <t>Kuchař naklonil nad umyvadlo</t>
+  </si>
+  <si>
+    <t>Petr zapsal datum do sešitu</t>
+  </si>
+  <si>
+    <t>Petr se zapsal datum do sešitu</t>
+  </si>
+  <si>
+    <t>Petr se zapsal do sešitu</t>
+  </si>
+  <si>
+    <t>Petr zapsal do sešitu</t>
+  </si>
+  <si>
+    <t>Maminka vzbudila dceru brzo ráno</t>
+  </si>
+  <si>
+    <t>Maminka se vzbudila dceru brzo ráno</t>
+  </si>
+  <si>
+    <t>Maminka se vzbudila brzo ráno</t>
+  </si>
+  <si>
+    <t>Maminka vzbudila brzo ráno</t>
+  </si>
+  <si>
+    <t>Tchýně trápila rodinu hladem</t>
+  </si>
+  <si>
+    <t>Tchýně se trápila rodinu hladem</t>
+  </si>
+  <si>
+    <t>Tchýně se trápila hladem</t>
+  </si>
+  <si>
+    <t>Tchýně trápila hladem</t>
+  </si>
+  <si>
+    <t>Plavec ponořil hlavu pod vodu</t>
+  </si>
+  <si>
+    <t>Plavec se ponořil hlavu pod vodu</t>
+  </si>
+  <si>
+    <t>Plavec se ponořil pod vodu</t>
+  </si>
+  <si>
+    <t>Plavec ponořil pod vodu</t>
+  </si>
+  <si>
+    <t>Trenér stáhnul fotbalistu z hřiště</t>
+  </si>
+  <si>
+    <t>Trenér se stáhnul fotbalistu z hřiště</t>
+  </si>
+  <si>
+    <t>Trenér se stáhnul z hřiště</t>
+  </si>
+  <si>
+    <t>Trenér stáhnul z hřiště</t>
+  </si>
+  <si>
+    <t>neměla by být i zácvičná část</t>
+  </si>
+  <si>
+    <t>Výrobce prezentoval produkt jako lepší alternativu</t>
+  </si>
+  <si>
+    <t>Výrobce se prezentoval produkt jako lepší alternativu</t>
+  </si>
+  <si>
+    <t>Výrobce se prezentoval jako lepší alternativa</t>
+  </si>
+  <si>
+    <t>Výrobce prezentoval jako lepší alternativa</t>
+  </si>
+  <si>
+    <t>Sekretářka ohlásila příchod (návštěvy) v telefonu</t>
+  </si>
+  <si>
+    <t>Podnikatel hájil svůj postup před soudem</t>
+  </si>
+  <si>
+    <t>Podnikatel se hájil svůj postup před soudem</t>
+  </si>
+  <si>
+    <t>Podnikatel se hájil před soudem</t>
+  </si>
+  <si>
+    <t>Podnikatel hájil před soudem</t>
+  </si>
+  <si>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>group2</t>
+  </si>
+  <si>
+    <t>Předseda hájil zájmy zaměstnanců před komisí</t>
+  </si>
+  <si>
+    <t>Předseda se hájil zájmy zaměstnanců před komisí</t>
+  </si>
+  <si>
+    <t>Předseda se hájil před komisí</t>
+  </si>
+  <si>
+    <t>Předseda hájil před komisí</t>
+  </si>
+  <si>
+    <t>Pilot ohlásil přílet přes vysílačku</t>
+  </si>
+  <si>
+    <t>Pilot se ohlásil přes vysílačku</t>
+  </si>
+  <si>
+    <t>Pilot se ohlásil přílet přes vysílačku</t>
+  </si>
+  <si>
+    <t>Pilot ohlásil přes vysílačku</t>
+  </si>
+  <si>
+    <t>Tým prezentoval projekt jako rychlé řešení problému</t>
+  </si>
+  <si>
+    <t>Tým se prezentoval projekt jako rychlé řešení problému</t>
+  </si>
+  <si>
+    <t>Tým se prezentoval jako rychlé řešení problému</t>
+  </si>
+  <si>
+    <t>Tým prezentoval jako rychlé řešení problému</t>
+  </si>
+  <si>
+    <t>Agentura stáhla léky z trhu</t>
+  </si>
+  <si>
+    <t>Agentura se stáhla léky z trhu</t>
+  </si>
+  <si>
+    <t>Agentura se stáhla z trhu</t>
+  </si>
+  <si>
+    <t>Agentura stáhla z trhu</t>
+  </si>
+  <si>
+    <t>Delfín ponořil ocas pod hladinu</t>
+  </si>
+  <si>
+    <t>Delfín se ponořil ocas pod hladinu</t>
+  </si>
+  <si>
+    <t>Delfín se ponořil pod hladinu</t>
+  </si>
+  <si>
+    <t>Delfín ponořil pod hladinu</t>
+  </si>
+  <si>
+    <t>Starosta trápil obyvatele svým znovuzvolením</t>
+  </si>
+  <si>
+    <t>Starosta se trápil svým znovuzvolením</t>
+  </si>
+  <si>
+    <t>Starosta se trápil obyvatele svým znovuzvolením</t>
+  </si>
+  <si>
+    <t>Starosta trápil svým znovuzvolením</t>
+  </si>
+  <si>
+    <t>Tomáš vzbudil sousedy příliš pozdě</t>
+  </si>
+  <si>
+    <t>Tomáš se vzbudil sousedy příliš pozdě</t>
+  </si>
+  <si>
+    <t>Tomáš se vzbudil příliš pozdě</t>
+  </si>
+  <si>
+    <t>Tomáš vzbudil příliš pozdě</t>
+  </si>
+  <si>
+    <t>Vrátník zapsal datum do kalendáře</t>
+  </si>
+  <si>
+    <t>Vrátník se zapsal datum do kalendáře</t>
+  </si>
+  <si>
+    <t>Vrátník se zapsal do kalendáře</t>
+  </si>
+  <si>
+    <t>Vrátník zapsal do kalendáře</t>
+  </si>
+  <si>
+    <t>Pavel naklonil hlavu ke straně</t>
+  </si>
+  <si>
+    <t>Pavel se naklonil hlavu ke straně</t>
+  </si>
+  <si>
+    <t>Pavel se naklonil ke straně</t>
+  </si>
+  <si>
+    <t>Pavel naklonil ke straně</t>
+  </si>
+  <si>
+    <t>Vedoucí omluvil neúčast zaměstnance na schůzce</t>
+  </si>
+  <si>
+    <t>Vedoucí se omluvil neúčast zaměstnance na schůzce</t>
+  </si>
+  <si>
+    <t>Vedoucí se omluvil na schůzce</t>
+  </si>
+  <si>
+    <t>Vedoucí omluvil na schůzce</t>
+  </si>
+  <si>
+    <t>Strýček přestěhoval svou rodinu z Polska</t>
+  </si>
+  <si>
+    <t>Strýček se přestěhoval svou rodinu z Polska</t>
+  </si>
+  <si>
+    <t>Strýček se přestěhoval z Polska</t>
+  </si>
+  <si>
+    <t>Strýček přestěhoval z Polska</t>
+  </si>
+  <si>
+    <t>Moderátor rozesmál účinkující na jevišti</t>
+  </si>
+  <si>
+    <t>Moderátor se rozesmál účinkující na jevišti</t>
+  </si>
+  <si>
+    <t>Moderátor se rozesmál na jevišti</t>
+  </si>
+  <si>
+    <t>Moderátor rozesmál na jevišti</t>
+  </si>
+  <si>
+    <t>Ondřej vypravil děti do školy</t>
+  </si>
+  <si>
+    <t>Ondřej se vypravil děti do školy</t>
+  </si>
+  <si>
+    <t>Ondřej vypravil do školy</t>
+  </si>
+  <si>
+    <t>Ondřej se vypravil do školy</t>
+  </si>
+  <si>
+    <t>Vědci zaměřili své úsilí na výzkum spánku</t>
+  </si>
+  <si>
+    <t>Vědci se zaměřili své úsilí na výzkum spánku</t>
+  </si>
+  <si>
+    <t>Vědci se zaměřili na výzkum spánku</t>
+  </si>
+  <si>
+    <t>Vědci zaměřili na výzkum spánku</t>
+  </si>
+  <si>
+    <t>Lékař zbavil pacienta závislosti od alkoholu</t>
+  </si>
+  <si>
+    <t>Lékař se zbavil pacienta závislosti od alkoholu</t>
+  </si>
+  <si>
+    <t>Lékař se zbavil závislosti od alkoholu</t>
+  </si>
+  <si>
+    <t>Lékař zbavil závislosti od alkoholu</t>
+  </si>
+  <si>
+    <t>Lucie vzbudila Moniku až po snídani</t>
+  </si>
+  <si>
+    <t>Lucie se vzbudila Moniku až po snídani</t>
+  </si>
+  <si>
+    <t>Lucie se vzbudila až po snídani</t>
+  </si>
+  <si>
+    <t>Lucie vzbudila až po snídani</t>
+  </si>
+  <si>
+    <t>Dědeček se probudil vnuka v devět hodin</t>
+  </si>
+  <si>
+    <t>Psycholog zbavil přebytečného stresu</t>
+  </si>
+  <si>
+    <t>Psycholog zbavil klienta přebytečného stresu</t>
+  </si>
+  <si>
+    <t>Psycholog se zbavil klienta přebytečného stresu</t>
+  </si>
+  <si>
+    <t>Psycholog se zbavil přebytečného stresu</t>
+  </si>
+  <si>
+    <t>Sekretářka ohlásila v telefonu</t>
+  </si>
+  <si>
+    <t>Sekretářka se ohlásila v telefonu</t>
+  </si>
+  <si>
+    <t>Herec rozesmál publikum až na konci představení</t>
+  </si>
+  <si>
+    <t>Herec se rozesmál publikum až na konci představení</t>
+  </si>
+  <si>
+    <t>Herec se rozesmál až na konci představení</t>
+  </si>
+  <si>
+    <t>Herec rozesmál až na konci představení</t>
+  </si>
+  <si>
+    <t>Kuchař naklonil hrnec nad umyvadlo</t>
+  </si>
+  <si>
+    <t>Kuchař se naklonil hrnec nad umyvadlo</t>
+  </si>
+  <si>
+    <t>Sekretářka se ohlásila příchod (návštěvy) v telefonu</t>
+  </si>
+  <si>
+    <t>Má být morfologická podoba slovesa vždy stejná?</t>
   </si>
 </sst>
 </file>
@@ -712,10 +1079,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1003,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,7 +1381,7 @@
     <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1056,13 +1422,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1082,22 +1448,16 @@
       <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
-        <v>148</v>
-      </c>
-      <c r="K2" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1118,21 +1478,21 @@
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1153,21 +1513,21 @@
         <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -1188,21 +1548,21 @@
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1214,30 +1574,30 @@
         <v>0</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="K6" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -1258,21 +1618,21 @@
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -1284,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="s">
         <v>3</v>
@@ -1293,21 +1653,21 @@
         <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -1316,10 +1676,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
         <v>3</v>
@@ -1328,21 +1688,21 @@
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -1354,30 +1714,30 @@
         <v>0</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="I10" t="s">
         <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="K10" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -1386,33 +1746,33 @@
         <v>0</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="I11" t="s">
         <v>4</v>
       </c>
       <c r="J11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="K11" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -1424,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="s">
         <v>17</v>
@@ -1433,21 +1793,21 @@
         <v>4</v>
       </c>
       <c r="J12" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="K12" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1459,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
@@ -1468,21 +1828,21 @@
         <v>4</v>
       </c>
       <c r="J13" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="K13" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -1494,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="s">
         <v>17</v>
@@ -1503,21 +1863,21 @@
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="K14" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -1538,21 +1898,21 @@
         <v>4</v>
       </c>
       <c r="J15" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="K15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -1573,21 +1933,21 @@
         <v>4</v>
       </c>
       <c r="J16" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="K16" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -1608,155 +1968,15 @@
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="K17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J18" t="s">
-        <v>112</v>
-      </c>
-      <c r="K18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" t="s">
-        <v>110</v>
-      </c>
-      <c r="K19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" t="s">
-        <v>108</v>
-      </c>
-      <c r="K20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" t="s">
-        <v>106</v>
-      </c>
-      <c r="K21" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>164</v>
+      <c r="A32" s="8" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1964,13 +2184,13 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -1985,21 +2205,27 @@
         <v>0</v>
       </c>
       <c r="H40" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="I40" t="s">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="J40" t="s">
+        <v>120</v>
+      </c>
+      <c r="K40" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -2017,24 +2243,24 @@
         <v>17</v>
       </c>
       <c r="I41" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="J41" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -2055,9 +2281,149 @@
         <v>4</v>
       </c>
       <c r="J42" t="s">
+        <v>141</v>
+      </c>
+      <c r="K42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" t="s">
+        <v>136</v>
+      </c>
+      <c r="K43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" t="s">
+        <v>3</v>
+      </c>
+      <c r="I44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" t="s">
+        <v>148</v>
+      </c>
+      <c r="K44" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" t="s">
+        <v>3</v>
+      </c>
+      <c r="I45" t="s">
+        <v>4</v>
+      </c>
+      <c r="J45" t="s">
+        <v>146</v>
+      </c>
+      <c r="K45" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" t="s">
+        <v>102</v>
+      </c>
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" t="s">
+        <v>3</v>
+      </c>
+      <c r="I47" t="s">
+        <v>4</v>
+      </c>
+      <c r="J47" t="s">
         <v>128</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K47" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2067,251 +2433,693 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174360F2-0B0E-4EF1-A5CC-2464ACF992AE}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057030CB-B800-4519-95A3-3E74CCF461EF}">
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="C2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="B4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057030CB-B800-4519-95A3-3E74CCF461EF}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="D5" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D9" t="s">
+        <v>293</v>
+      </c>
+      <c r="E9" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C12" t="s">
+        <v>301</v>
+      </c>
+      <c r="D12" t="s">
+        <v>298</v>
+      </c>
+      <c r="E12" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" t="s">
+        <v>302</v>
+      </c>
+      <c r="E15" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
+        <v>197</v>
+      </c>
+      <c r="C16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" t="s">
+        <v>195</v>
+      </c>
+      <c r="E16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" t="s">
+        <v>210</v>
+      </c>
+      <c r="D19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" t="s">
+        <v>211</v>
+      </c>
+      <c r="E20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C21" t="s">
+        <v>219</v>
+      </c>
+      <c r="D21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>297</v>
+      </c>
+      <c r="C22" t="s">
+        <v>296</v>
+      </c>
+      <c r="D22" t="s">
+        <v>220</v>
+      </c>
+      <c r="E22" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D23" t="s">
+        <v>221</v>
+      </c>
+      <c r="E23" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B25" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="C25" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="D25" t="s">
         <v>169</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E25" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>173</v>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>289</v>
+      </c>
+      <c r="C26" t="s">
+        <v>290</v>
+      </c>
+      <c r="D26" t="s">
+        <v>287</v>
+      </c>
+      <c r="E26" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>285</v>
+      </c>
+      <c r="C27" t="s">
+        <v>286</v>
+      </c>
+      <c r="D27" t="s">
+        <v>283</v>
+      </c>
+      <c r="E27" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>281</v>
+      </c>
+      <c r="C28" t="s">
+        <v>282</v>
+      </c>
+      <c r="D28" t="s">
+        <v>279</v>
+      </c>
+      <c r="E28" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>278</v>
+      </c>
+      <c r="C29" t="s">
+        <v>277</v>
+      </c>
+      <c r="D29" t="s">
+        <v>275</v>
+      </c>
+      <c r="E29" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>273</v>
+      </c>
+      <c r="C30" t="s">
+        <v>274</v>
+      </c>
+      <c r="D30" t="s">
+        <v>271</v>
+      </c>
+      <c r="E30" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>269</v>
+      </c>
+      <c r="C31" t="s">
+        <v>270</v>
+      </c>
+      <c r="D31" t="s">
+        <v>267</v>
+      </c>
+      <c r="E31" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>265</v>
+      </c>
+      <c r="C32" t="s">
+        <v>266</v>
+      </c>
+      <c r="D32" t="s">
+        <v>263</v>
+      </c>
+      <c r="E32" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>261</v>
+      </c>
+      <c r="C33" t="s">
+        <v>262</v>
+      </c>
+      <c r="D33" t="s">
+        <v>259</v>
+      </c>
+      <c r="E33" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s">
+        <v>257</v>
+      </c>
+      <c r="C34" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" t="s">
+        <v>255</v>
+      </c>
+      <c r="E34" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>253</v>
+      </c>
+      <c r="C35" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" t="s">
+        <v>251</v>
+      </c>
+      <c r="E35" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" t="s">
+        <v>248</v>
+      </c>
+      <c r="C36" t="s">
+        <v>250</v>
+      </c>
+      <c r="D36" t="s">
+        <v>247</v>
+      </c>
+      <c r="E36" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" t="s">
+        <v>246</v>
+      </c>
+      <c r="D37" t="s">
+        <v>243</v>
+      </c>
+      <c r="E37" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" t="s">
+        <v>241</v>
+      </c>
+      <c r="C38" t="s">
+        <v>242</v>
+      </c>
+      <c r="D38" t="s">
+        <v>239</v>
+      </c>
+      <c r="E38" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>237</v>
+      </c>
+      <c r="C39" t="s">
+        <v>238</v>
+      </c>
+      <c r="D39" t="s">
+        <v>235</v>
+      </c>
+      <c r="E39" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" t="s">
+        <v>231</v>
+      </c>
+      <c r="E40" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>229</v>
+      </c>
+      <c r="C41" t="s">
+        <v>230</v>
+      </c>
+      <c r="D41" t="s">
+        <v>227</v>
+      </c>
+      <c r="E41" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E30DFC-42CC-4AC5-B31A-93F0F62B75CA}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
results of preliminary experiment
</commit_message>
<xml_diff>
--- a/corpus/final_lemmas.xlsx
+++ b/corpus/final_lemmas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user1\materialy\bc\reflexive-alternation-in-aphasia\corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA99D6DD-890D-47A2-96A6-27367071ED52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3D59A6-B427-4C2D-93F4-C7CC09D669B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lemmas" sheetId="1" r:id="rId1"/>
@@ -569,18 +569,6 @@
     <t>Generál se spojil s nepřítelem</t>
   </si>
   <si>
-    <t>Prezident spojil Česko se zahraničím</t>
-  </si>
-  <si>
-    <t>Prezident se spojil se zahraničím</t>
-  </si>
-  <si>
-    <t>Prezident se spojil Česko se zahraničím</t>
-  </si>
-  <si>
-    <t>Prezident spojil se zahraničím</t>
-  </si>
-  <si>
     <t>Generál se spojil síly s nepřítelem</t>
   </si>
   <si>
@@ -599,18 +587,6 @@
     <t>Herec rozesmál po představení</t>
   </si>
   <si>
-    <t>Úředník zaměřil pozornost na práci</t>
-  </si>
-  <si>
-    <t>Úředník se zaměřil pozornost na práci</t>
-  </si>
-  <si>
-    <t>Úředník zaměřil na práci</t>
-  </si>
-  <si>
-    <t>Úředník se zaměřil na práci</t>
-  </si>
-  <si>
     <t>Psycholog zbavil klienta stresu</t>
   </si>
   <si>
@@ -623,12 +599,6 @@
     <t>Psycholog zbavil stresu</t>
   </si>
   <si>
-    <t>Podnikatel hájil postup před soudem</t>
-  </si>
-  <si>
-    <t>Podnikatel se hájil postup před soudem</t>
-  </si>
-  <si>
     <t>Předseda hájil zaměstnance před komisí</t>
   </si>
   <si>
@@ -767,66 +737,6 @@
     <t>Dělník se přestěhoval nábytek do bytu</t>
   </si>
   <si>
-    <t>Policista se vzbudil pozdě</t>
-  </si>
-  <si>
-    <t>Policista vzbudil pozdě</t>
-  </si>
-  <si>
-    <t>Policista vzbudil sousedy pozdě</t>
-  </si>
-  <si>
-    <t>Policista se vzbudil sousedy pozdě</t>
-  </si>
-  <si>
-    <t>Tatínek se vzbudil ráno</t>
-  </si>
-  <si>
-    <t>Tatínek vzbudil ráno</t>
-  </si>
-  <si>
-    <t>Tatínek vzbudil dceru ráno</t>
-  </si>
-  <si>
-    <t>Tatínek se vzbudil dceru ráno</t>
-  </si>
-  <si>
-    <t>Vedoucí se oddělil od skupiny</t>
-  </si>
-  <si>
-    <t>Vedoucí oddělil od skupiny</t>
-  </si>
-  <si>
-    <t>Vedoucí oddělil děti od skupiny</t>
-  </si>
-  <si>
-    <t>Vedoucí se oddělil děti od skupiny</t>
-  </si>
-  <si>
-    <t>Učitel probudil žáky ve třídě</t>
-  </si>
-  <si>
-    <t>Učitel se probudil žáky ve třídě</t>
-  </si>
-  <si>
-    <t>Učitel se probudil ve třídě</t>
-  </si>
-  <si>
-    <t>Učitel probudil ve třídě</t>
-  </si>
-  <si>
-    <t>Soutěžící se ponořil pod hladinu</t>
-  </si>
-  <si>
-    <t>Soutěžící ponořil pod hladinu</t>
-  </si>
-  <si>
-    <t>Soutěžící ponořil obličej pod hladinu</t>
-  </si>
-  <si>
-    <t>Soutěžící se ponořil obličej pod hladinu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lékař se zbavil závislosti </t>
   </si>
   <si>
@@ -849,6 +759,96 @@
   </si>
   <si>
     <t>Trenér se stáhl fotbalistu z hřiště</t>
+  </si>
+  <si>
+    <t>Tatínek se vzbudil včas</t>
+  </si>
+  <si>
+    <t>Tatínek vzbudil včas</t>
+  </si>
+  <si>
+    <t>Tatínek vzbudil dceru včas</t>
+  </si>
+  <si>
+    <t>Tatínek se vzbudil dceru včas</t>
+  </si>
+  <si>
+    <t>Učitel se oddělil od skupiny</t>
+  </si>
+  <si>
+    <t>Učitel oddělil od skupiny</t>
+  </si>
+  <si>
+    <t>Učitel oddělil děti od skupiny</t>
+  </si>
+  <si>
+    <t>Učitel se oddělil děti od skupiny</t>
+  </si>
+  <si>
+    <t>Podnikatel hájil firmu před soudem</t>
+  </si>
+  <si>
+    <t>Podnikatel se hájil firmu před soudem</t>
+  </si>
+  <si>
+    <t>Úředník se zaměřil na stížnost</t>
+  </si>
+  <si>
+    <t>Úředník zaměřil na stížnost</t>
+  </si>
+  <si>
+    <t>Úředník zaměřil pozornost na stížnost</t>
+  </si>
+  <si>
+    <t>Úředník se zaměřil pozornost na stížnost</t>
+  </si>
+  <si>
+    <t>Kancléř spojil prezidenta s ministrem.</t>
+  </si>
+  <si>
+    <t>Kancléř se spojil prezidenta s ministrem.</t>
+  </si>
+  <si>
+    <t>Kancléř se spojil s ministrem</t>
+  </si>
+  <si>
+    <t>Kancléř spojil s ministrem</t>
+  </si>
+  <si>
+    <t>Tatínek se vzbudil pozdě</t>
+  </si>
+  <si>
+    <t>Tatínek vzbudil pozdě</t>
+  </si>
+  <si>
+    <t>Tatínek vzbudil sousedy pozdě</t>
+  </si>
+  <si>
+    <t>Tatínek se vzbudil sousedy pozdě</t>
+  </si>
+  <si>
+    <t>Opilec probudil kamaráda na konečné</t>
+  </si>
+  <si>
+    <t>Opilec se probudil kamaráda na konečné</t>
+  </si>
+  <si>
+    <t>Opilec se probudil na konečné</t>
+  </si>
+  <si>
+    <t>Opilec probudil na konečné</t>
+  </si>
+  <si>
+    <t>Sportovec se ponořil pod hladinu</t>
+  </si>
+  <si>
+    <t>Sportovec ponořil pod hladinu</t>
+  </si>
+  <si>
+    <t>Sportovec ponořil obličej pod hladinu</t>
+  </si>
+  <si>
+    <t>Sportovec se ponořil obličej pod hladinu</t>
   </si>
 </sst>
 </file>
@@ -1175,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H42" sqref="A42:H44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2175,8 +2175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057030CB-B800-4519-95A3-3E74CCF461EF}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="B2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2257,16 +2257,16 @@
         <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="E4" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="F4" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2277,16 +2277,16 @@
         <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2317,16 +2317,16 @@
         <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>253</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>254</v>
       </c>
       <c r="E7" t="s">
-        <v>189</v>
+        <v>255</v>
       </c>
       <c r="F7" t="s">
-        <v>190</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2337,16 +2337,16 @@
         <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D8" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E8" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F8" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2383,10 +2383,10 @@
         <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>251</v>
       </c>
       <c r="F10" t="s">
-        <v>198</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2397,16 +2397,16 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="D11" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E11" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="F11" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2417,16 +2417,16 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E12" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F12" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2437,16 +2437,16 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
       <c r="D13" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="E13" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="F13" t="s">
-        <v>272</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2457,16 +2457,16 @@
         <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D14" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="E14" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="F14" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2477,16 +2477,16 @@
         <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D15" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E15" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F15" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2497,16 +2497,16 @@
         <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D16" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E16" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="F16" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2520,13 +2520,13 @@
         <v>178</v>
       </c>
       <c r="D17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E17" t="s">
         <v>177</v>
       </c>
       <c r="F17" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2539,8 +2539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218EE2FB-CC5D-4679-8DB0-1D2BBF936312}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2581,16 +2581,16 @@
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="D2" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E2" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="F2" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2601,16 +2601,16 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D3" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="E3" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="F3" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2621,16 +2621,16 @@
         <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="E4" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="F4" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2661,16 +2661,16 @@
         <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="E6" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="F6" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2681,16 +2681,16 @@
         <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E7" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2701,16 +2701,16 @@
         <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="D8" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="E8" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
       <c r="F8" t="s">
-        <v>268</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2721,16 +2721,16 @@
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="D9" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E9" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="F9" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2747,10 +2747,10 @@
         <v>160</v>
       </c>
       <c r="E10" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="F10" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2801,16 +2801,16 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D13" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="E13" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F13" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2821,16 +2821,16 @@
         <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D14" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="E14" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="F14" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2841,16 +2841,16 @@
         <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="D15" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="E15" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="F15" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2861,16 +2861,16 @@
         <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D16" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="E16" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F16" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2881,16 +2881,16 @@
         <v>176</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>259</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>260</v>
       </c>
       <c r="E17" t="s">
-        <v>179</v>
+        <v>257</v>
       </c>
       <c r="F17" t="s">
-        <v>181</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change the most problematic sentences
</commit_message>
<xml_diff>
--- a/corpus/final_lemmas.xlsx
+++ b/corpus/final_lemmas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user1\materialy\bc\reflexive-alternation-in-aphasia\corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3D59A6-B427-4C2D-93F4-C7CC09D669B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B790452-5078-4750-8E9A-F47D9F17712E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lemmas" sheetId="1" r:id="rId1"/>
@@ -641,30 +641,6 @@
     <t>Číšník se trápil hosty hladem</t>
   </si>
   <si>
-    <t>Student se zapsal do sešitu</t>
-  </si>
-  <si>
-    <t>Student zapsal do sešitu</t>
-  </si>
-  <si>
-    <t>Student zapsal datum do sešitu</t>
-  </si>
-  <si>
-    <t>Student se zapsal datum do sešitu</t>
-  </si>
-  <si>
-    <t>Vrátný se zapsal do kalendáře</t>
-  </si>
-  <si>
-    <t>Vrátný zapsal do kalendáře</t>
-  </si>
-  <si>
-    <t>Vrátný zapsal datum do kalendáře</t>
-  </si>
-  <si>
-    <t>Vrátný se zapsal datum do kalendáře</t>
-  </si>
-  <si>
     <t>Výrobce se stáhl z trhu</t>
   </si>
   <si>
@@ -849,6 +825,30 @@
   </si>
   <si>
     <t>Sportovec se ponořil obličej pod hladinu</t>
+  </si>
+  <si>
+    <t>Vrátný zapsal návštěvu u vchodu</t>
+  </si>
+  <si>
+    <t>Vrátný se zapsal návštěvu u vchodu</t>
+  </si>
+  <si>
+    <t>Vrátný se zapsal u vchodu</t>
+  </si>
+  <si>
+    <t>Vrátný zapsal u vchodu</t>
+  </si>
+  <si>
+    <t>Student zapsal výsledky při odchodu</t>
+  </si>
+  <si>
+    <t>Student se zapsal výsledky při odchodu</t>
+  </si>
+  <si>
+    <t>Student se zapsal při odchodu</t>
+  </si>
+  <si>
+    <t>Student zapsal při odchodu</t>
   </si>
 </sst>
 </file>
@@ -864,7 +864,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -874,6 +874,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -890,9 +896,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2175,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057030CB-B800-4519-95A3-3E74CCF461EF}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="B2:F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2257,16 +2264,16 @@
         <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E4" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F4" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2317,16 +2324,16 @@
         <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D7" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E7" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="F7" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2379,14 +2386,14 @@
       <c r="C10" t="s">
         <v>157</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="F10" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2417,16 +2424,16 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D12" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E12" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F12" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2437,16 +2444,16 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D13" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E13" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F13" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2477,16 +2484,16 @@
         <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D15" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E15" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F15" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2497,16 +2504,16 @@
         <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>203</v>
+        <v>271</v>
       </c>
       <c r="D16" t="s">
-        <v>204</v>
+        <v>272</v>
       </c>
       <c r="E16" t="s">
-        <v>205</v>
+        <v>269</v>
       </c>
       <c r="F16" t="s">
-        <v>206</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2539,8 +2546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218EE2FB-CC5D-4679-8DB0-1D2BBF936312}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2581,16 +2588,16 @@
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D2" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="E2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="F2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2601,16 +2608,16 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D3" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E3" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="F3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2621,16 +2628,16 @@
         <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E4" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F4" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2661,16 +2668,16 @@
         <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D6" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E6" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F6" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2681,16 +2688,16 @@
         <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E7" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="F7" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2701,16 +2708,16 @@
         <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D8" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E8" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F8" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2721,16 +2728,16 @@
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="D9" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="E9" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="F9" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2743,7 +2750,7 @@
       <c r="C10" t="s">
         <v>159</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E10" t="s">
@@ -2763,7 +2770,7 @@
       <c r="C11" t="s">
         <v>162</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>164</v>
       </c>
       <c r="E11" t="s">
@@ -2783,7 +2790,7 @@
       <c r="C12" t="s">
         <v>174</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>175</v>
       </c>
       <c r="E12" t="s">
@@ -2801,16 +2808,16 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D13" t="s">
-        <v>212</v>
+        <v>203</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="E13" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F13" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2823,7 +2830,7 @@
       <c r="C14" t="s">
         <v>191</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>192</v>
       </c>
       <c r="E14" t="s">
@@ -2841,16 +2848,16 @@
         <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>261</v>
-      </c>
-      <c r="D15" t="s">
-        <v>262</v>
+        <v>253</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="E15" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="F15" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2861,16 +2868,16 @@
         <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
-      </c>
-      <c r="D16" t="s">
-        <v>208</v>
+        <v>267</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="E16" t="s">
-        <v>209</v>
+        <v>265</v>
       </c>
       <c r="F16" t="s">
-        <v>210</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2881,16 +2888,16 @@
         <v>176</v>
       </c>
       <c r="C17" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D17" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E17" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="F17" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>